<commit_message>
final with tests and visualisations
</commit_message>
<xml_diff>
--- a/Serve_Cleaned.xlsx
+++ b/Serve_Cleaned.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G351"/>
+  <dimension ref="A1:G354"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -5928,7 +5928,7 @@
     </row>
     <row r="178">
       <c r="A178" t="n">
-        <v>14.48</v>
+        <v>17.89</v>
       </c>
       <c r="B178" t="n">
         <v>2</v>
@@ -5959,14 +5959,14 @@
     </row>
     <row r="179">
       <c r="A179" t="n">
-        <v>96.59999999999999</v>
+        <v>14.48</v>
       </c>
       <c r="B179" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C179" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D179" t="inlineStr">
@@ -5990,14 +5990,14 @@
     </row>
     <row r="180">
       <c r="A180" t="n">
-        <v>34.63</v>
+        <v>96.59999999999999</v>
       </c>
       <c r="B180" t="n">
-        <v>3.55</v>
+        <v>4</v>
       </c>
       <c r="C180" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D180" t="inlineStr">
@@ -6021,10 +6021,10 @@
     </row>
     <row r="181">
       <c r="A181" t="n">
-        <v>34.65</v>
+        <v>34.63</v>
       </c>
       <c r="B181" t="n">
-        <v>3.68</v>
+        <v>3.55</v>
       </c>
       <c r="C181" t="inlineStr">
         <is>
@@ -6047,15 +6047,15 @@
         </is>
       </c>
       <c r="G181" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="182">
       <c r="A182" t="n">
-        <v>23.33</v>
+        <v>34.65</v>
       </c>
       <c r="B182" t="n">
-        <v>5.65</v>
+        <v>3.68</v>
       </c>
       <c r="C182" t="inlineStr">
         <is>
@@ -6078,15 +6078,15 @@
         </is>
       </c>
       <c r="G182" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="183">
       <c r="A183" t="n">
-        <v>45.35</v>
+        <v>23.33</v>
       </c>
       <c r="B183" t="n">
-        <v>3.5</v>
+        <v>5.65</v>
       </c>
       <c r="C183" t="inlineStr">
         <is>
@@ -6109,15 +6109,15 @@
         </is>
       </c>
       <c r="G183" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="184">
       <c r="A184" t="n">
-        <v>23.17</v>
+        <v>45.35</v>
       </c>
       <c r="B184" t="n">
-        <v>6.5</v>
+        <v>3.5</v>
       </c>
       <c r="C184" t="inlineStr">
         <is>
@@ -6140,15 +6140,15 @@
         </is>
       </c>
       <c r="G184" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="185">
       <c r="A185" t="n">
-        <v>40.55</v>
+        <v>23.17</v>
       </c>
       <c r="B185" t="n">
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="C185" t="inlineStr">
         <is>
@@ -6171,15 +6171,15 @@
         </is>
       </c>
       <c r="G185" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="186">
       <c r="A186" t="n">
-        <v>20.69</v>
+        <v>40.55</v>
       </c>
       <c r="B186" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="C186" t="inlineStr">
         <is>
@@ -6188,7 +6188,7 @@
       </c>
       <c r="D186" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E186" t="inlineStr">
@@ -6202,19 +6202,19 @@
         </is>
       </c>
       <c r="G186" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
     </row>
     <row r="187">
       <c r="A187" t="n">
-        <v>20.9</v>
+        <v>20.69</v>
       </c>
       <c r="B187" t="n">
-        <v>3.5</v>
+        <v>5</v>
       </c>
       <c r="C187" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D187" t="inlineStr">
@@ -6233,29 +6233,29 @@
         </is>
       </c>
       <c r="G187" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="188">
       <c r="A188" t="n">
-        <v>30.46</v>
+        <v>20.9</v>
       </c>
       <c r="B188" t="n">
-        <v>2</v>
+        <v>3.5</v>
       </c>
       <c r="C188" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D188" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E188" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F188" t="inlineStr">
@@ -6264,19 +6264,19 @@
         </is>
       </c>
       <c r="G188" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="189">
       <c r="A189" t="n">
-        <v>18.15</v>
+        <v>30.46</v>
       </c>
       <c r="B189" t="n">
-        <v>3.5</v>
+        <v>2</v>
       </c>
       <c r="C189" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D189" t="inlineStr">
@@ -6286,7 +6286,7 @@
       </c>
       <c r="E189" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F189" t="inlineStr">
@@ -6295,19 +6295,19 @@
         </is>
       </c>
       <c r="G189" t="n">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="190">
       <c r="A190" t="n">
-        <v>23.1</v>
+        <v>18.15</v>
       </c>
       <c r="B190" t="n">
-        <v>4</v>
+        <v>3.5</v>
       </c>
       <c r="C190" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D190" t="inlineStr">
@@ -6331,10 +6331,10 @@
     </row>
     <row r="191">
       <c r="A191" t="n">
-        <v>15.69</v>
+        <v>23.1</v>
       </c>
       <c r="B191" t="n">
-        <v>1.5</v>
+        <v>4</v>
       </c>
       <c r="C191" t="inlineStr">
         <is>
@@ -6357,19 +6357,19 @@
         </is>
       </c>
       <c r="G191" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" t="n">
-        <v>19.81</v>
+        <v>15.69</v>
       </c>
       <c r="B192" t="n">
-        <v>4.19</v>
+        <v>1.5</v>
       </c>
       <c r="C192" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D192" t="inlineStr">
@@ -6379,12 +6379,12 @@
       </c>
       <c r="E192" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F192" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G192" t="n">
@@ -6393,14 +6393,14 @@
     </row>
     <row r="193">
       <c r="A193" t="n">
-        <v>28.44</v>
+        <v>19.81</v>
       </c>
       <c r="B193" t="n">
-        <v>2.56</v>
+        <v>4.19</v>
       </c>
       <c r="C193" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D193" t="inlineStr">
@@ -6424,10 +6424,10 @@
     </row>
     <row r="194">
       <c r="A194" t="n">
-        <v>15.48</v>
+        <v>28.44</v>
       </c>
       <c r="B194" t="n">
-        <v>2.02</v>
+        <v>2.56</v>
       </c>
       <c r="C194" t="inlineStr">
         <is>
@@ -6450,15 +6450,15 @@
         </is>
       </c>
       <c r="G194" t="n">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="195">
       <c r="A195" t="n">
-        <v>16.58</v>
+        <v>15.48</v>
       </c>
       <c r="B195" t="n">
-        <v>4</v>
+        <v>2.02</v>
       </c>
       <c r="C195" t="inlineStr">
         <is>
@@ -6481,15 +6481,15 @@
         </is>
       </c>
       <c r="G195" t="n">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="196">
       <c r="A196" t="n">
-        <v>7.56</v>
+        <v>16.58</v>
       </c>
       <c r="B196" t="n">
-        <v>1.44</v>
+        <v>4</v>
       </c>
       <c r="C196" t="inlineStr">
         <is>
@@ -6498,7 +6498,7 @@
       </c>
       <c r="D196" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E196" t="inlineStr">
@@ -6517,10 +6517,10 @@
     </row>
     <row r="197">
       <c r="A197" t="n">
-        <v>10.34</v>
+        <v>7.56</v>
       </c>
       <c r="B197" t="n">
-        <v>2</v>
+        <v>1.44</v>
       </c>
       <c r="C197" t="inlineStr">
         <is>
@@ -6529,7 +6529,7 @@
       </c>
       <c r="D197" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E197" t="inlineStr">
@@ -6579,14 +6579,14 @@
     </row>
     <row r="199">
       <c r="A199" t="n">
-        <v>43.11</v>
+        <v>10.34</v>
       </c>
       <c r="B199" t="n">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C199" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D199" t="inlineStr">
@@ -6605,19 +6605,19 @@
         </is>
       </c>
       <c r="G199" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="200">
       <c r="A200" t="n">
-        <v>13.51</v>
+        <v>43.11</v>
       </c>
       <c r="B200" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C200" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D200" t="inlineStr">
@@ -6636,19 +6636,19 @@
         </is>
       </c>
       <c r="G200" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="201">
       <c r="A201" t="n">
-        <v>18.71</v>
+        <v>13</v>
       </c>
       <c r="B201" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C201" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D201" t="inlineStr">
@@ -6667,19 +6667,19 @@
         </is>
       </c>
       <c r="G201" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="202">
       <c r="A202" t="n">
-        <v>12.74</v>
+        <v>13.51</v>
       </c>
       <c r="B202" t="n">
-        <v>2.01</v>
+        <v>2</v>
       </c>
       <c r="C202" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D202" t="inlineStr">
@@ -6703,14 +6703,14 @@
     </row>
     <row r="203">
       <c r="A203" t="n">
-        <v>13</v>
+        <v>18.71</v>
       </c>
       <c r="B203" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C203" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D203" t="inlineStr">
@@ -6729,15 +6729,15 @@
         </is>
       </c>
       <c r="G203" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="204">
       <c r="A204" t="n">
-        <v>16.4</v>
+        <v>12.74</v>
       </c>
       <c r="B204" t="n">
-        <v>2.5</v>
+        <v>2.01</v>
       </c>
       <c r="C204" t="inlineStr">
         <is>
@@ -6765,14 +6765,14 @@
     </row>
     <row r="205">
       <c r="A205" t="n">
-        <v>20.53</v>
+        <v>13</v>
       </c>
       <c r="B205" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C205" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D205" t="inlineStr">
@@ -6791,15 +6791,15 @@
         </is>
       </c>
       <c r="G205" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="206">
       <c r="A206" t="n">
-        <v>16.47</v>
+        <v>16.4</v>
       </c>
       <c r="B206" t="n">
-        <v>3.23</v>
+        <v>2.5</v>
       </c>
       <c r="C206" t="inlineStr">
         <is>
@@ -6822,15 +6822,15 @@
         </is>
       </c>
       <c r="G206" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="207">
       <c r="A207" t="n">
-        <v>26.59</v>
+        <v>20.53</v>
       </c>
       <c r="B207" t="n">
-        <v>3.41</v>
+        <v>4</v>
       </c>
       <c r="C207" t="inlineStr">
         <is>
@@ -6844,28 +6844,28 @@
       </c>
       <c r="E207" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F207" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G207" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="208">
       <c r="A208" t="n">
-        <v>38.73</v>
+        <v>16.47</v>
       </c>
       <c r="B208" t="n">
-        <v>3</v>
+        <v>3.23</v>
       </c>
       <c r="C208" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D208" t="inlineStr">
@@ -6875,24 +6875,24 @@
       </c>
       <c r="E208" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F208" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G208" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="209">
       <c r="A209" t="n">
-        <v>24.27</v>
+        <v>26.59</v>
       </c>
       <c r="B209" t="n">
-        <v>2.03</v>
+        <v>3.41</v>
       </c>
       <c r="C209" t="inlineStr">
         <is>
@@ -6915,19 +6915,19 @@
         </is>
       </c>
       <c r="G209" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="210">
       <c r="A210" t="n">
-        <v>12.76</v>
+        <v>38.73</v>
       </c>
       <c r="B210" t="n">
-        <v>2.23</v>
+        <v>3</v>
       </c>
       <c r="C210" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D210" t="inlineStr">
@@ -6946,15 +6946,15 @@
         </is>
       </c>
       <c r="G210" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="211">
       <c r="A211" t="n">
-        <v>30.06</v>
+        <v>24.27</v>
       </c>
       <c r="B211" t="n">
-        <v>2</v>
+        <v>2.03</v>
       </c>
       <c r="C211" t="inlineStr">
         <is>
@@ -6977,19 +6977,19 @@
         </is>
       </c>
       <c r="G211" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="212">
       <c r="A212" t="n">
-        <v>25.89</v>
+        <v>12.76</v>
       </c>
       <c r="B212" t="n">
-        <v>5.16</v>
+        <v>2.23</v>
       </c>
       <c r="C212" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D212" t="inlineStr">
@@ -7008,15 +7008,15 @@
         </is>
       </c>
       <c r="G212" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="213">
       <c r="A213" t="n">
-        <v>48.33</v>
+        <v>30.06</v>
       </c>
       <c r="B213" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="C213" t="inlineStr">
         <is>
@@ -7025,7 +7025,7 @@
       </c>
       <c r="D213" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E213" t="inlineStr">
@@ -7039,19 +7039,19 @@
         </is>
       </c>
       <c r="G213" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="214">
       <c r="A214" t="n">
-        <v>13.27</v>
+        <v>25.89</v>
       </c>
       <c r="B214" t="n">
-        <v>2.5</v>
+        <v>5.16</v>
       </c>
       <c r="C214" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D214" t="inlineStr">
@@ -7070,24 +7070,24 @@
         </is>
       </c>
       <c r="G214" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="215">
       <c r="A215" t="n">
-        <v>28.17</v>
+        <v>48.33</v>
       </c>
       <c r="B215" t="n">
-        <v>6.5</v>
+        <v>9</v>
       </c>
       <c r="C215" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D215" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E215" t="inlineStr">
@@ -7101,15 +7101,15 @@
         </is>
       </c>
       <c r="G215" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="216">
       <c r="A216" t="n">
-        <v>12.9</v>
+        <v>13.27</v>
       </c>
       <c r="B216" t="n">
-        <v>1.1</v>
+        <v>2.5</v>
       </c>
       <c r="C216" t="inlineStr">
         <is>
@@ -7137,14 +7137,14 @@
     </row>
     <row r="217">
       <c r="A217" t="n">
-        <v>28.15</v>
+        <v>28.17</v>
       </c>
       <c r="B217" t="n">
-        <v>3</v>
+        <v>6.5</v>
       </c>
       <c r="C217" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D217" t="inlineStr">
@@ -7163,19 +7163,19 @@
         </is>
       </c>
       <c r="G217" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="218">
       <c r="A218" t="n">
-        <v>11.59</v>
+        <v>12.9</v>
       </c>
       <c r="B218" t="n">
-        <v>1.5</v>
+        <v>1.1</v>
       </c>
       <c r="C218" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D218" t="inlineStr">
@@ -7199,10 +7199,10 @@
     </row>
     <row r="219">
       <c r="A219" t="n">
-        <v>7.74</v>
+        <v>28.15</v>
       </c>
       <c r="B219" t="n">
-        <v>1.44</v>
+        <v>3</v>
       </c>
       <c r="C219" t="inlineStr">
         <is>
@@ -7225,15 +7225,15 @@
         </is>
       </c>
       <c r="G219" t="n">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="220">
       <c r="A220" t="n">
-        <v>12.16</v>
+        <v>11.59</v>
       </c>
       <c r="B220" t="n">
-        <v>2.2</v>
+        <v>1.5</v>
       </c>
       <c r="C220" t="inlineStr">
         <is>
@@ -7247,12 +7247,12 @@
       </c>
       <c r="E220" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F220" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G220" t="n">
@@ -7261,14 +7261,14 @@
     </row>
     <row r="221">
       <c r="A221" t="n">
-        <v>13.42</v>
+        <v>7.74</v>
       </c>
       <c r="B221" t="n">
-        <v>3.48</v>
+        <v>1.44</v>
       </c>
       <c r="C221" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D221" t="inlineStr">
@@ -7278,12 +7278,12 @@
       </c>
       <c r="E221" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F221" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G221" t="n">
@@ -7292,14 +7292,14 @@
     </row>
     <row r="222">
       <c r="A222" t="n">
-        <v>8.58</v>
+        <v>30.14</v>
       </c>
       <c r="B222" t="n">
-        <v>1.92</v>
+        <v>3.09</v>
       </c>
       <c r="C222" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D222" t="inlineStr">
@@ -7309,33 +7309,33 @@
       </c>
       <c r="E222" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F222" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G222" t="n">
-        <v>1</v>
+        <v>4</v>
       </c>
     </row>
     <row r="223">
       <c r="A223" t="n">
-        <v>15.98</v>
+        <v>12.16</v>
       </c>
       <c r="B223" t="n">
-        <v>3</v>
+        <v>2.2</v>
       </c>
       <c r="C223" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D223" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E223" t="inlineStr">
@@ -7349,7 +7349,7 @@
         </is>
       </c>
       <c r="G223" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="224">
@@ -7357,11 +7357,11 @@
         <v>13.42</v>
       </c>
       <c r="B224" t="n">
-        <v>1.58</v>
+        <v>3.48</v>
       </c>
       <c r="C224" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D224" t="inlineStr">
@@ -7385,14 +7385,14 @@
     </row>
     <row r="225">
       <c r="A225" t="n">
-        <v>16.27</v>
+        <v>8.58</v>
       </c>
       <c r="B225" t="n">
-        <v>2.5</v>
+        <v>1.92</v>
       </c>
       <c r="C225" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D225" t="inlineStr">
@@ -7411,15 +7411,15 @@
         </is>
       </c>
       <c r="G225" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="226">
       <c r="A226" t="n">
-        <v>10.09</v>
+        <v>15.98</v>
       </c>
       <c r="B226" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C226" t="inlineStr">
         <is>
@@ -7428,7 +7428,7 @@
       </c>
       <c r="D226" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E226" t="inlineStr">
@@ -7442,15 +7442,15 @@
         </is>
       </c>
       <c r="G226" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="227">
       <c r="A227" t="n">
-        <v>20.45</v>
+        <v>13.42</v>
       </c>
       <c r="B227" t="n">
-        <v>3</v>
+        <v>1.58</v>
       </c>
       <c r="C227" t="inlineStr">
         <is>
@@ -7459,48 +7459,48 @@
       </c>
       <c r="D227" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E227" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F227" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G227" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="228">
       <c r="A228" t="n">
-        <v>13.28</v>
+        <v>16.27</v>
       </c>
       <c r="B228" t="n">
-        <v>2.72</v>
+        <v>2.5</v>
       </c>
       <c r="C228" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D228" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E228" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F228" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G228" t="n">
@@ -7509,10 +7509,10 @@
     </row>
     <row r="229">
       <c r="A229" t="n">
-        <v>22.12</v>
+        <v>10.09</v>
       </c>
       <c r="B229" t="n">
-        <v>2.88</v>
+        <v>2</v>
       </c>
       <c r="C229" t="inlineStr">
         <is>
@@ -7526,12 +7526,12 @@
       </c>
       <c r="E229" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F229" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G229" t="n">
@@ -7540,10 +7540,10 @@
     </row>
     <row r="230">
       <c r="A230" t="n">
-        <v>24.01</v>
+        <v>20.45</v>
       </c>
       <c r="B230" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C230" t="inlineStr">
         <is>
@@ -7552,7 +7552,7 @@
       </c>
       <c r="D230" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E230" t="inlineStr">
@@ -7571,10 +7571,10 @@
     </row>
     <row r="231">
       <c r="A231" t="n">
-        <v>15.69</v>
+        <v>13.28</v>
       </c>
       <c r="B231" t="n">
-        <v>3</v>
+        <v>2.72</v>
       </c>
       <c r="C231" t="inlineStr">
         <is>
@@ -7583,7 +7583,7 @@
       </c>
       <c r="D231" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E231" t="inlineStr">
@@ -7597,24 +7597,24 @@
         </is>
       </c>
       <c r="G231" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="232">
       <c r="A232" t="n">
-        <v>11.61</v>
+        <v>22.12</v>
       </c>
       <c r="B232" t="n">
-        <v>3.39</v>
+        <v>2.88</v>
       </c>
       <c r="C232" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D232" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E232" t="inlineStr">
@@ -7633,10 +7633,10 @@
     </row>
     <row r="233">
       <c r="A233" t="n">
-        <v>10.77</v>
+        <v>24.01</v>
       </c>
       <c r="B233" t="n">
-        <v>1.47</v>
+        <v>2</v>
       </c>
       <c r="C233" t="inlineStr">
         <is>
@@ -7645,7 +7645,7 @@
       </c>
       <c r="D233" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E233" t="inlineStr">
@@ -7659,12 +7659,12 @@
         </is>
       </c>
       <c r="G233" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="234">
       <c r="A234" t="n">
-        <v>15.53</v>
+        <v>15.69</v>
       </c>
       <c r="B234" t="n">
         <v>3</v>
@@ -7690,15 +7690,15 @@
         </is>
       </c>
       <c r="G234" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="235">
       <c r="A235" t="n">
-        <v>10.07</v>
+        <v>11.61</v>
       </c>
       <c r="B235" t="n">
-        <v>1.25</v>
+        <v>3.39</v>
       </c>
       <c r="C235" t="inlineStr">
         <is>
@@ -7726,10 +7726,10 @@
     </row>
     <row r="236">
       <c r="A236" t="n">
-        <v>12.6</v>
+        <v>10.77</v>
       </c>
       <c r="B236" t="n">
-        <v>1</v>
+        <v>1.47</v>
       </c>
       <c r="C236" t="inlineStr">
         <is>
@@ -7738,7 +7738,7 @@
       </c>
       <c r="D236" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E236" t="inlineStr">
@@ -7757,10 +7757,10 @@
     </row>
     <row r="237">
       <c r="A237" t="n">
-        <v>32.83</v>
+        <v>15.53</v>
       </c>
       <c r="B237" t="n">
-        <v>1.17</v>
+        <v>3</v>
       </c>
       <c r="C237" t="inlineStr">
         <is>
@@ -7788,14 +7788,14 @@
     </row>
     <row r="238">
       <c r="A238" t="n">
-        <v>35.83</v>
+        <v>10.07</v>
       </c>
       <c r="B238" t="n">
-        <v>4.67</v>
+        <v>1.25</v>
       </c>
       <c r="C238" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D238" t="inlineStr">
@@ -7814,15 +7814,15 @@
         </is>
       </c>
       <c r="G238" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="239">
       <c r="A239" t="n">
-        <v>29.03</v>
+        <v>12.6</v>
       </c>
       <c r="B239" t="n">
-        <v>5.92</v>
+        <v>1</v>
       </c>
       <c r="C239" t="inlineStr">
         <is>
@@ -7831,7 +7831,7 @@
       </c>
       <c r="D239" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E239" t="inlineStr">
@@ -7845,19 +7845,19 @@
         </is>
       </c>
       <c r="G239" t="n">
-        <v>38</v>
+        <v>2</v>
       </c>
     </row>
     <row r="240">
       <c r="A240" t="n">
-        <v>27.18</v>
+        <v>32.83</v>
       </c>
       <c r="B240" t="n">
-        <v>2</v>
+        <v>1.17</v>
       </c>
       <c r="C240" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D240" t="inlineStr">
@@ -7881,19 +7881,19 @@
     </row>
     <row r="241">
       <c r="A241" t="n">
-        <v>22.67</v>
+        <v>35.83</v>
       </c>
       <c r="B241" t="n">
-        <v>2</v>
+        <v>4.67</v>
       </c>
       <c r="C241" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D241" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E241" t="inlineStr">
@@ -7907,15 +7907,15 @@
         </is>
       </c>
       <c r="G241" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="242">
       <c r="A242" t="n">
-        <v>17.82</v>
+        <v>29.03</v>
       </c>
       <c r="B242" t="n">
-        <v>1.75</v>
+        <v>5.92</v>
       </c>
       <c r="C242" t="inlineStr">
         <is>
@@ -7938,15 +7938,15 @@
         </is>
       </c>
       <c r="G242" t="n">
-        <v>2</v>
+        <v>38</v>
       </c>
     </row>
     <row r="243">
       <c r="A243" t="n">
-        <v>18.78</v>
+        <v>27.18</v>
       </c>
       <c r="B243" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C243" t="inlineStr">
         <is>
@@ -7955,12 +7955,12 @@
       </c>
       <c r="D243" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E243" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F243" t="inlineStr">
@@ -7974,10 +7974,10 @@
     </row>
     <row r="244">
       <c r="A244" t="n">
-        <v>19.29</v>
+        <v>22.67</v>
       </c>
       <c r="B244" t="n">
-        <v>3.23</v>
+        <v>2</v>
       </c>
       <c r="C244" t="inlineStr">
         <is>
@@ -7991,7 +7991,7 @@
       </c>
       <c r="E244" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F244" t="inlineStr">
@@ -8000,19 +8000,19 @@
         </is>
       </c>
       <c r="G244" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="245">
       <c r="A245" t="n">
-        <v>26.34</v>
+        <v>17.82</v>
       </c>
       <c r="B245" t="n">
-        <v>4.12</v>
+        <v>1.75</v>
       </c>
       <c r="C245" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D245" t="inlineStr">
@@ -8027,19 +8027,19 @@
       </c>
       <c r="F245" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G245" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="246">
       <c r="A246" t="n">
-        <v>24.21</v>
+        <v>18.78</v>
       </c>
       <c r="B246" t="n">
-        <v>3.19</v>
+        <v>3</v>
       </c>
       <c r="C246" t="inlineStr">
         <is>
@@ -8053,7 +8053,7 @@
       </c>
       <c r="E246" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F246" t="inlineStr">
@@ -8067,14 +8067,14 @@
     </row>
     <row r="247">
       <c r="A247" t="n">
-        <v>18.23</v>
+        <v>19.29</v>
       </c>
       <c r="B247" t="n">
-        <v>2.18</v>
+        <v>3.23</v>
       </c>
       <c r="C247" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D247" t="inlineStr">
@@ -8084,12 +8084,12 @@
       </c>
       <c r="E247" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F247" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G247" t="n">
@@ -8098,19 +8098,19 @@
     </row>
     <row r="248">
       <c r="A248" t="n">
-        <v>20.5</v>
+        <v>26.34</v>
       </c>
       <c r="B248" t="n">
-        <v>2.1</v>
+        <v>4.12</v>
       </c>
       <c r="C248" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D248" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E248" t="inlineStr">
@@ -8120,28 +8120,28 @@
       </c>
       <c r="F248" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G248" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="249">
       <c r="A249" t="n">
-        <v>30.87</v>
+        <v>24.21</v>
       </c>
       <c r="B249" t="n">
-        <v>3.69</v>
+        <v>3.19</v>
       </c>
       <c r="C249" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D249" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E249" t="inlineStr">
@@ -8151,19 +8151,19 @@
       </c>
       <c r="F249" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G249" t="n">
-        <v>29</v>
+        <v>2</v>
       </c>
     </row>
     <row r="250">
       <c r="A250" t="n">
-        <v>24.56</v>
+        <v>18.23</v>
       </c>
       <c r="B250" t="n">
-        <v>2.88</v>
+        <v>2.18</v>
       </c>
       <c r="C250" t="inlineStr">
         <is>
@@ -8172,12 +8172,12 @@
       </c>
       <c r="D250" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E250" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F250" t="inlineStr">
@@ -8186,19 +8186,19 @@
         </is>
       </c>
       <c r="G250" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="251">
       <c r="A251" t="n">
-        <v>13.69</v>
+        <v>20.5</v>
       </c>
       <c r="B251" t="n">
-        <v>2</v>
+        <v>2.1</v>
       </c>
       <c r="C251" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D251" t="inlineStr">
@@ -8208,12 +8208,12 @@
       </c>
       <c r="E251" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F251" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G251" t="n">
@@ -8222,10 +8222,10 @@
     </row>
     <row r="252">
       <c r="A252" t="n">
-        <v>17.89</v>
+        <v>30.87</v>
       </c>
       <c r="B252" t="n">
-        <v>2.98</v>
+        <v>3.69</v>
       </c>
       <c r="C252" t="inlineStr">
         <is>
@@ -8239,24 +8239,24 @@
       </c>
       <c r="E252" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F252" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G252" t="n">
-        <v>3</v>
+        <v>29</v>
       </c>
     </row>
     <row r="253">
       <c r="A253" t="n">
-        <v>22.89</v>
+        <v>24.56</v>
       </c>
       <c r="B253" t="n">
-        <v>3</v>
+        <v>2.88</v>
       </c>
       <c r="C253" t="inlineStr">
         <is>
@@ -8270,12 +8270,12 @@
       </c>
       <c r="E253" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F253" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G253" t="n">
@@ -8284,24 +8284,24 @@
     </row>
     <row r="254">
       <c r="A254" t="n">
-        <v>19.1</v>
+        <v>13.69</v>
       </c>
       <c r="B254" t="n">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="C254" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D254" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E254" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F254" t="inlineStr">
@@ -8315,55 +8315,55 @@
     </row>
     <row r="255">
       <c r="A255" t="n">
-        <v>9.869999999999999</v>
+        <v>17.89</v>
       </c>
       <c r="B255" t="n">
-        <v>1.68</v>
+        <v>2.98</v>
       </c>
       <c r="C255" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D255" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E255" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F255" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G255" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="256">
       <c r="A256" t="n">
-        <v>19.65</v>
+        <v>22.89</v>
       </c>
       <c r="B256" t="n">
-        <v>2.89</v>
+        <v>3</v>
       </c>
       <c r="C256" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D256" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E256" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F256" t="inlineStr">
@@ -8377,19 +8377,19 @@
     </row>
     <row r="257">
       <c r="A257" t="n">
-        <v>25.68</v>
+        <v>19.1</v>
       </c>
       <c r="B257" t="n">
-        <v>3.87</v>
+        <v>3.1</v>
       </c>
       <c r="C257" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D257" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E257" t="inlineStr">
@@ -8403,15 +8403,15 @@
         </is>
       </c>
       <c r="G257" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="258">
       <c r="A258" t="n">
-        <v>33.87</v>
+        <v>9.869999999999999</v>
       </c>
       <c r="B258" t="n">
-        <v>4</v>
+        <v>1.68</v>
       </c>
       <c r="C258" t="inlineStr">
         <is>
@@ -8425,7 +8425,7 @@
       </c>
       <c r="E258" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F258" t="inlineStr">
@@ -8434,15 +8434,15 @@
         </is>
       </c>
       <c r="G258" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
     </row>
     <row r="259">
       <c r="A259" t="n">
-        <v>40.45</v>
+        <v>19.65</v>
       </c>
       <c r="B259" t="n">
-        <v>4.85</v>
+        <v>2.89</v>
       </c>
       <c r="C259" t="inlineStr">
         <is>
@@ -8456,7 +8456,7 @@
       </c>
       <c r="E259" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F259" t="inlineStr">
@@ -8465,15 +8465,15 @@
         </is>
       </c>
       <c r="G259" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="260">
       <c r="A260" t="n">
-        <v>33.76</v>
+        <v>25.68</v>
       </c>
       <c r="B260" t="n">
-        <v>3.29</v>
+        <v>3.87</v>
       </c>
       <c r="C260" t="inlineStr">
         <is>
@@ -8482,7 +8482,7 @@
       </c>
       <c r="D260" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E260" t="inlineStr">
@@ -8492,7 +8492,7 @@
       </c>
       <c r="F260" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G260" t="n">
@@ -8501,10 +8501,10 @@
     </row>
     <row r="261">
       <c r="A261" t="n">
-        <v>29.87</v>
+        <v>33.87</v>
       </c>
       <c r="B261" t="n">
-        <v>3.7</v>
+        <v>4</v>
       </c>
       <c r="C261" t="inlineStr">
         <is>
@@ -8523,23 +8523,23 @@
       </c>
       <c r="F261" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G261" t="n">
-        <v>45</v>
+        <v>4</v>
       </c>
     </row>
     <row r="262">
       <c r="A262" t="n">
-        <v>18.98</v>
+        <v>40.45</v>
       </c>
       <c r="B262" t="n">
-        <v>1.8</v>
+        <v>4.85</v>
       </c>
       <c r="C262" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D262" t="inlineStr">
@@ -8549,38 +8549,38 @@
       </c>
       <c r="E262" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F262" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G262" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="263">
       <c r="A263" t="n">
-        <v>8.880000000000001</v>
+        <v>33.76</v>
       </c>
       <c r="B263" t="n">
-        <v>1.5</v>
+        <v>3.29</v>
       </c>
       <c r="C263" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D263" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E263" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F263" t="inlineStr">
@@ -8589,15 +8589,15 @@
         </is>
       </c>
       <c r="G263" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="264">
       <c r="A264" t="n">
-        <v>13.89</v>
+        <v>29.87</v>
       </c>
       <c r="B264" t="n">
-        <v>2.38</v>
+        <v>3.7</v>
       </c>
       <c r="C264" t="inlineStr">
         <is>
@@ -8611,24 +8611,24 @@
       </c>
       <c r="E264" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F264" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G264" t="n">
-        <v>2</v>
+        <v>45</v>
       </c>
     </row>
     <row r="265">
       <c r="A265" t="n">
-        <v>29.99</v>
+        <v>18.98</v>
       </c>
       <c r="B265" t="n">
-        <v>3.39</v>
+        <v>1.8</v>
       </c>
       <c r="C265" t="inlineStr">
         <is>
@@ -8637,29 +8637,29 @@
       </c>
       <c r="D265" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E265" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F265" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G265" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="266">
       <c r="A266" t="n">
-        <v>43.8</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="B266" t="n">
-        <v>4.39</v>
+        <v>1.5</v>
       </c>
       <c r="C266" t="inlineStr">
         <is>
@@ -8673,28 +8673,28 @@
       </c>
       <c r="E266" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F266" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G266" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="267">
       <c r="A267" t="n">
-        <v>8.9</v>
+        <v>13.89</v>
       </c>
       <c r="B267" t="n">
-        <v>1.5</v>
+        <v>2.38</v>
       </c>
       <c r="C267" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D267" t="inlineStr">
@@ -8713,24 +8713,24 @@
         </is>
       </c>
       <c r="G267" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="268">
       <c r="A268" t="n">
-        <v>23.91</v>
+        <v>29.99</v>
       </c>
       <c r="B268" t="n">
-        <v>2.65</v>
+        <v>3.39</v>
       </c>
       <c r="C268" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D268" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E268" t="inlineStr">
@@ -8744,34 +8744,34 @@
         </is>
       </c>
       <c r="G268" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="269">
       <c r="A269" t="n">
-        <v>33.8</v>
+        <v>43.8</v>
       </c>
       <c r="B269" t="n">
-        <v>3</v>
+        <v>4.39</v>
       </c>
       <c r="C269" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D269" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E269" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F269" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G269" t="n">
@@ -8780,24 +8780,24 @@
     </row>
     <row r="270">
       <c r="A270" t="n">
-        <v>40.9</v>
+        <v>8.9</v>
       </c>
       <c r="B270" t="n">
-        <v>4.67</v>
+        <v>1.5</v>
       </c>
       <c r="C270" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D270" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E270" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F270" t="inlineStr">
@@ -8806,15 +8806,15 @@
         </is>
       </c>
       <c r="G270" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="271">
       <c r="A271" t="n">
-        <v>22.66</v>
+        <v>23.91</v>
       </c>
       <c r="B271" t="n">
-        <v>2.5</v>
+        <v>2.65</v>
       </c>
       <c r="C271" t="inlineStr">
         <is>
@@ -8823,26 +8823,26 @@
       </c>
       <c r="D271" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E271" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F271" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G271" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="272">
       <c r="A272" t="n">
-        <v>29.76</v>
+        <v>33.8</v>
       </c>
       <c r="B272" t="n">
         <v>3</v>
@@ -8859,12 +8859,12 @@
       </c>
       <c r="E272" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F272" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G272" t="n">
@@ -8873,10 +8873,10 @@
     </row>
     <row r="273">
       <c r="A273" t="n">
-        <v>15</v>
+        <v>40.9</v>
       </c>
       <c r="B273" t="n">
-        <v>2.5</v>
+        <v>4.67</v>
       </c>
       <c r="C273" t="inlineStr">
         <is>
@@ -8895,19 +8895,19 @@
       </c>
       <c r="F273" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G273" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="274">
       <c r="A274" t="n">
-        <v>22.5</v>
+        <v>22.66</v>
       </c>
       <c r="B274" t="n">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="C274" t="inlineStr">
         <is>
@@ -8921,7 +8921,7 @@
       </c>
       <c r="E274" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F274" t="inlineStr">
@@ -8935,14 +8935,14 @@
     </row>
     <row r="275">
       <c r="A275" t="n">
-        <v>33.6</v>
+        <v>29.76</v>
       </c>
       <c r="B275" t="n">
         <v>3</v>
       </c>
       <c r="C275" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D275" t="inlineStr">
@@ -8952,24 +8952,24 @@
       </c>
       <c r="E275" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F275" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G275" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="276">
       <c r="A276" t="n">
-        <v>25.65</v>
+        <v>15</v>
       </c>
       <c r="B276" t="n">
-        <v>2.56</v>
+        <v>2.5</v>
       </c>
       <c r="C276" t="inlineStr">
         <is>
@@ -8988,7 +8988,7 @@
       </c>
       <c r="F276" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G276" t="n">
@@ -8997,14 +8997,14 @@
     </row>
     <row r="277">
       <c r="A277" t="n">
-        <v>30</v>
+        <v>22.5</v>
       </c>
       <c r="B277" t="n">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="C277" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D277" t="inlineStr">
@@ -9014,7 +9014,7 @@
       </c>
       <c r="E277" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F277" t="inlineStr">
@@ -9028,10 +9028,10 @@
     </row>
     <row r="278">
       <c r="A278" t="n">
-        <v>16.7</v>
+        <v>33.6</v>
       </c>
       <c r="B278" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="C278" t="inlineStr">
         <is>
@@ -9040,12 +9040,12 @@
       </c>
       <c r="D278" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E278" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F278" t="inlineStr">
@@ -9059,10 +9059,10 @@
     </row>
     <row r="279">
       <c r="A279" t="n">
-        <v>25.55</v>
+        <v>25.65</v>
       </c>
       <c r="B279" t="n">
-        <v>2.3</v>
+        <v>2.56</v>
       </c>
       <c r="C279" t="inlineStr">
         <is>
@@ -9071,12 +9071,12 @@
       </c>
       <c r="D279" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E279" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F279" t="inlineStr">
@@ -9085,15 +9085,15 @@
         </is>
       </c>
       <c r="G279" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="280">
       <c r="A280" t="n">
-        <v>27.79</v>
+        <v>30</v>
       </c>
       <c r="B280" t="n">
-        <v>2.59</v>
+        <v>3</v>
       </c>
       <c r="C280" t="inlineStr">
         <is>
@@ -9107,24 +9107,24 @@
       </c>
       <c r="E280" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F280" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G280" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="281">
       <c r="A281" t="n">
-        <v>30.3</v>
+        <v>16.7</v>
       </c>
       <c r="B281" t="n">
-        <v>2.15</v>
+        <v>1.5</v>
       </c>
       <c r="C281" t="inlineStr">
         <is>
@@ -9147,15 +9147,15 @@
         </is>
       </c>
       <c r="G281" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="282">
       <c r="A282" t="n">
-        <v>10.1</v>
+        <v>25.55</v>
       </c>
       <c r="B282" t="n">
-        <v>1.8</v>
+        <v>2.3</v>
       </c>
       <c r="C282" t="inlineStr">
         <is>
@@ -9169,7 +9169,7 @@
       </c>
       <c r="E282" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F282" t="inlineStr">
@@ -9178,15 +9178,15 @@
         </is>
       </c>
       <c r="G282" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="283">
       <c r="A283" t="n">
-        <v>16.68</v>
+        <v>27.79</v>
       </c>
       <c r="B283" t="n">
-        <v>1.9</v>
+        <v>2.59</v>
       </c>
       <c r="C283" t="inlineStr">
         <is>
@@ -9195,7 +9195,7 @@
       </c>
       <c r="D283" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E283" t="inlineStr">
@@ -9214,14 +9214,14 @@
     </row>
     <row r="284">
       <c r="A284" t="n">
-        <v>16.68</v>
+        <v>30.3</v>
       </c>
       <c r="B284" t="n">
-        <v>1.9</v>
+        <v>2.15</v>
       </c>
       <c r="C284" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D284" t="inlineStr">
@@ -9231,7 +9231,7 @@
       </c>
       <c r="E284" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F284" t="inlineStr">
@@ -9240,29 +9240,29 @@
         </is>
       </c>
       <c r="G284" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="285">
       <c r="A285" t="n">
-        <v>19.9</v>
+        <v>10.1</v>
       </c>
       <c r="B285" t="n">
-        <v>2</v>
+        <v>1.8</v>
       </c>
       <c r="C285" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D285" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E285" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F285" t="inlineStr">
@@ -9276,10 +9276,10 @@
     </row>
     <row r="286">
       <c r="A286" t="n">
-        <v>30.35</v>
+        <v>16.68</v>
       </c>
       <c r="B286" t="n">
-        <v>3.3</v>
+        <v>1.9</v>
       </c>
       <c r="C286" t="inlineStr">
         <is>
@@ -9288,7 +9288,7 @@
       </c>
       <c r="D286" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E286" t="inlineStr">
@@ -9298,23 +9298,23 @@
       </c>
       <c r="F286" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G286" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="287">
       <c r="A287" t="n">
-        <v>44.34</v>
+        <v>16.68</v>
       </c>
       <c r="B287" t="n">
-        <v>4.1</v>
+        <v>1.9</v>
       </c>
       <c r="C287" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D287" t="inlineStr">
@@ -9333,15 +9333,15 @@
         </is>
       </c>
       <c r="G287" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" t="n">
-        <v>23.45</v>
+        <v>19.9</v>
       </c>
       <c r="B288" t="n">
-        <v>2.4</v>
+        <v>2</v>
       </c>
       <c r="C288" t="inlineStr">
         <is>
@@ -9350,12 +9350,12 @@
       </c>
       <c r="D288" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E288" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F288" t="inlineStr">
@@ -9369,10 +9369,10 @@
     </row>
     <row r="289">
       <c r="A289" t="n">
-        <v>17.7</v>
+        <v>30.35</v>
       </c>
       <c r="B289" t="n">
-        <v>2.35</v>
+        <v>3.3</v>
       </c>
       <c r="C289" t="inlineStr">
         <is>
@@ -9386,7 +9386,7 @@
       </c>
       <c r="E289" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F289" t="inlineStr">
@@ -9395,15 +9395,15 @@
         </is>
       </c>
       <c r="G289" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="290">
       <c r="A290" t="n">
-        <v>24.5</v>
+        <v>44.34</v>
       </c>
       <c r="B290" t="n">
-        <v>2.69</v>
+        <v>4.1</v>
       </c>
       <c r="C290" t="inlineStr">
         <is>
@@ -9412,48 +9412,48 @@
       </c>
       <c r="D290" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E290" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F290" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G290" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="291">
       <c r="A291" t="n">
-        <v>18</v>
+        <v>23.45</v>
       </c>
       <c r="B291" t="n">
-        <v>1.9</v>
+        <v>2.4</v>
       </c>
       <c r="C291" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D291" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E291" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F291" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G291" t="n">
@@ -9462,14 +9462,14 @@
     </row>
     <row r="292">
       <c r="A292" t="n">
-        <v>27.8</v>
+        <v>17.7</v>
       </c>
       <c r="B292" t="n">
-        <v>2.59</v>
+        <v>2.35</v>
       </c>
       <c r="C292" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D292" t="inlineStr">
@@ -9479,7 +9479,7 @@
       </c>
       <c r="E292" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F292" t="inlineStr">
@@ -9488,15 +9488,15 @@
         </is>
       </c>
       <c r="G292" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="293">
       <c r="A293" t="n">
-        <v>35.6</v>
+        <v>24.5</v>
       </c>
       <c r="B293" t="n">
-        <v>13.55</v>
+        <v>2.69</v>
       </c>
       <c r="C293" t="inlineStr">
         <is>
@@ -9515,7 +9515,7 @@
       </c>
       <c r="F293" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G293" t="n">
@@ -9524,10 +9524,10 @@
     </row>
     <row r="294">
       <c r="A294" t="n">
-        <v>29.9</v>
+        <v>18</v>
       </c>
       <c r="B294" t="n">
-        <v>2.1</v>
+        <v>1.9</v>
       </c>
       <c r="C294" t="inlineStr">
         <is>
@@ -9536,60 +9536,60 @@
       </c>
       <c r="D294" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E294" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F294" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G294" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="295">
       <c r="A295" t="n">
-        <v>16.57</v>
+        <v>27.8</v>
       </c>
       <c r="B295" t="n">
-        <v>1.79</v>
+        <v>2.59</v>
       </c>
       <c r="C295" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D295" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E295" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F295" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G295" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="296">
       <c r="A296" t="n">
-        <v>8.880000000000001</v>
+        <v>35.6</v>
       </c>
       <c r="B296" t="n">
-        <v>1</v>
+        <v>13.55</v>
       </c>
       <c r="C296" t="inlineStr">
         <is>
@@ -9598,7 +9598,7 @@
       </c>
       <c r="D296" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E296" t="inlineStr">
@@ -9608,23 +9608,23 @@
       </c>
       <c r="F296" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G296" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="297">
       <c r="A297" t="n">
-        <v>20.66</v>
+        <v>29.9</v>
       </c>
       <c r="B297" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="C297" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D297" t="inlineStr">
@@ -9634,24 +9634,24 @@
       </c>
       <c r="E297" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F297" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G297" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="298">
       <c r="A298" t="n">
-        <v>44.4</v>
+        <v>16.57</v>
       </c>
       <c r="B298" t="n">
-        <v>3.89</v>
+        <v>1.79</v>
       </c>
       <c r="C298" t="inlineStr">
         <is>
@@ -9660,7 +9660,7 @@
       </c>
       <c r="D298" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E298" t="inlineStr">
@@ -9670,23 +9670,23 @@
       </c>
       <c r="F298" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G298" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="299">
       <c r="A299" t="n">
-        <v>32.56</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="B299" t="n">
-        <v>2.96</v>
+        <v>1</v>
       </c>
       <c r="C299" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D299" t="inlineStr">
@@ -9696,7 +9696,7 @@
       </c>
       <c r="E299" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F299" t="inlineStr">
@@ -9705,15 +9705,15 @@
         </is>
       </c>
       <c r="G299" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="300">
       <c r="A300" t="n">
-        <v>27.8</v>
+        <v>20.66</v>
       </c>
       <c r="B300" t="n">
-        <v>2.59</v>
+        <v>1.9</v>
       </c>
       <c r="C300" t="inlineStr">
         <is>
@@ -9722,33 +9722,33 @@
       </c>
       <c r="D300" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E300" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F300" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G300" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="301">
       <c r="A301" t="n">
-        <v>35.6</v>
+        <v>44.4</v>
       </c>
       <c r="B301" t="n">
-        <v>3.55</v>
+        <v>3.89</v>
       </c>
       <c r="C301" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D301" t="inlineStr">
@@ -9758,12 +9758,12 @@
       </c>
       <c r="E301" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F301" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G301" t="n">
@@ -9772,10 +9772,10 @@
     </row>
     <row r="302">
       <c r="A302" t="n">
-        <v>29.9</v>
+        <v>32.56</v>
       </c>
       <c r="B302" t="n">
-        <v>2.1</v>
+        <v>2.96</v>
       </c>
       <c r="C302" t="inlineStr">
         <is>
@@ -9784,12 +9784,12 @@
       </c>
       <c r="D302" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E302" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F302" t="inlineStr">
@@ -9803,14 +9803,14 @@
     </row>
     <row r="303">
       <c r="A303" t="n">
-        <v>16.57</v>
+        <v>27.8</v>
       </c>
       <c r="B303" t="n">
-        <v>1.79</v>
+        <v>2.59</v>
       </c>
       <c r="C303" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D303" t="inlineStr">
@@ -9820,24 +9820,24 @@
       </c>
       <c r="E303" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F303" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G303" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="304">
       <c r="A304" t="n">
-        <v>8.880000000000001</v>
+        <v>35.6</v>
       </c>
       <c r="B304" t="n">
-        <v>1</v>
+        <v>3.55</v>
       </c>
       <c r="C304" t="inlineStr">
         <is>
@@ -9846,7 +9846,7 @@
       </c>
       <c r="D304" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E304" t="inlineStr">
@@ -9856,23 +9856,23 @@
       </c>
       <c r="F304" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G304" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="305">
       <c r="A305" t="n">
-        <v>20.66</v>
+        <v>29.9</v>
       </c>
       <c r="B305" t="n">
-        <v>1.9</v>
+        <v>2.1</v>
       </c>
       <c r="C305" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D305" t="inlineStr">
@@ -9882,24 +9882,24 @@
       </c>
       <c r="E305" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F305" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G305" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="306">
       <c r="A306" t="n">
-        <v>44.4</v>
+        <v>16.57</v>
       </c>
       <c r="B306" t="n">
-        <v>3.89</v>
+        <v>1.79</v>
       </c>
       <c r="C306" t="inlineStr">
         <is>
@@ -9908,7 +9908,7 @@
       </c>
       <c r="D306" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E306" t="inlineStr">
@@ -9918,23 +9918,23 @@
       </c>
       <c r="F306" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G306" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="307">
       <c r="A307" t="n">
-        <v>32.56</v>
+        <v>8.880000000000001</v>
       </c>
       <c r="B307" t="n">
-        <v>2.96</v>
+        <v>1</v>
       </c>
       <c r="C307" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D307" t="inlineStr">
@@ -9944,7 +9944,7 @@
       </c>
       <c r="E307" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F307" t="inlineStr">
@@ -9953,15 +9953,15 @@
         </is>
       </c>
       <c r="G307" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="308">
       <c r="A308" t="n">
-        <v>13.55</v>
+        <v>20.66</v>
       </c>
       <c r="B308" t="n">
-        <v>2.89</v>
+        <v>1.9</v>
       </c>
       <c r="C308" t="inlineStr">
         <is>
@@ -9975,7 +9975,7 @@
       </c>
       <c r="E308" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F308" t="inlineStr">
@@ -9984,19 +9984,19 @@
         </is>
       </c>
       <c r="G308" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="309">
       <c r="A309" t="n">
-        <v>11.43</v>
+        <v>44.4</v>
       </c>
       <c r="B309" t="n">
-        <v>1.47</v>
+        <v>3.89</v>
       </c>
       <c r="C309" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D309" t="inlineStr">
@@ -10006,7 +10006,7 @@
       </c>
       <c r="E309" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F309" t="inlineStr">
@@ -10015,19 +10015,19 @@
         </is>
       </c>
       <c r="G309" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" t="n">
-        <v>14.56</v>
+        <v>32.56</v>
       </c>
       <c r="B310" t="n">
-        <v>3.45</v>
+        <v>2.96</v>
       </c>
       <c r="C310" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D310" t="inlineStr">
@@ -10037,12 +10037,12 @@
       </c>
       <c r="E310" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F310" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G310" t="n">
@@ -10051,10 +10051,10 @@
     </row>
     <row r="311">
       <c r="A311" t="n">
-        <v>10.07</v>
+        <v>13.55</v>
       </c>
       <c r="B311" t="n">
-        <v>11.25</v>
+        <v>2.89</v>
       </c>
       <c r="C311" t="inlineStr">
         <is>
@@ -10077,19 +10077,19 @@
         </is>
       </c>
       <c r="G311" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="312">
       <c r="A312" t="n">
-        <v>22.01</v>
+        <v>11.43</v>
       </c>
       <c r="B312" t="n">
-        <v>3.23</v>
+        <v>1.47</v>
       </c>
       <c r="C312" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D312" t="inlineStr">
@@ -10099,7 +10099,7 @@
       </c>
       <c r="E312" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F312" t="inlineStr">
@@ -10113,14 +10113,14 @@
     </row>
     <row r="313">
       <c r="A313" t="n">
-        <v>13.69</v>
+        <v>14.56</v>
       </c>
       <c r="B313" t="n">
-        <v>2</v>
+        <v>3.45</v>
       </c>
       <c r="C313" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D313" t="inlineStr">
@@ -10130,24 +10130,24 @@
       </c>
       <c r="E313" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F313" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G313" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="314">
       <c r="A314" t="n">
-        <v>21.34</v>
+        <v>10.07</v>
       </c>
       <c r="B314" t="n">
-        <v>2.98</v>
+        <v>11.25</v>
       </c>
       <c r="C314" t="inlineStr">
         <is>
@@ -10156,12 +10156,12 @@
       </c>
       <c r="D314" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E314" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F314" t="inlineStr">
@@ -10170,15 +10170,15 @@
         </is>
       </c>
       <c r="G314" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="315">
       <c r="A315" t="n">
-        <v>12.89</v>
+        <v>22.01</v>
       </c>
       <c r="B315" t="n">
-        <v>3</v>
+        <v>3.23</v>
       </c>
       <c r="C315" t="inlineStr">
         <is>
@@ -10192,12 +10192,12 @@
       </c>
       <c r="E315" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F315" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G315" t="n">
@@ -10206,24 +10206,24 @@
     </row>
     <row r="316">
       <c r="A316" t="n">
-        <v>19.65</v>
+        <v>13.69</v>
       </c>
       <c r="B316" t="n">
-        <v>3.1</v>
+        <v>2</v>
       </c>
       <c r="C316" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D316" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E316" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F316" t="inlineStr">
@@ -10237,55 +10237,55 @@
     </row>
     <row r="317">
       <c r="A317" t="n">
-        <v>1.01</v>
+        <v>21.34</v>
       </c>
       <c r="B317" t="n">
-        <v>1.68</v>
+        <v>2.98</v>
       </c>
       <c r="C317" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D317" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E317" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F317" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G317" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="318">
       <c r="A318" t="n">
-        <v>19.65</v>
+        <v>12.89</v>
       </c>
       <c r="B318" t="n">
-        <v>2.09</v>
+        <v>3</v>
       </c>
       <c r="C318" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D318" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E318" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F318" t="inlineStr">
@@ -10299,19 +10299,19 @@
     </row>
     <row r="319">
       <c r="A319" t="n">
-        <v>21.56</v>
+        <v>19.65</v>
       </c>
       <c r="B319" t="n">
-        <v>3.66</v>
+        <v>3.1</v>
       </c>
       <c r="C319" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D319" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E319" t="inlineStr">
@@ -10325,15 +10325,15 @@
         </is>
       </c>
       <c r="G319" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="320">
       <c r="A320" t="n">
-        <v>28.87</v>
+        <v>1.01</v>
       </c>
       <c r="B320" t="n">
-        <v>3.67</v>
+        <v>1.68</v>
       </c>
       <c r="C320" t="inlineStr">
         <is>
@@ -10347,7 +10347,7 @@
       </c>
       <c r="E320" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F320" t="inlineStr">
@@ -10356,15 +10356,15 @@
         </is>
       </c>
       <c r="G320" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="321">
       <c r="A321" t="n">
-        <v>22.01</v>
+        <v>19.65</v>
       </c>
       <c r="B321" t="n">
-        <v>4</v>
+        <v>2.09</v>
       </c>
       <c r="C321" t="inlineStr">
         <is>
@@ -10378,7 +10378,7 @@
       </c>
       <c r="E321" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F321" t="inlineStr">
@@ -10387,24 +10387,24 @@
         </is>
       </c>
       <c r="G321" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="322">
       <c r="A322" t="n">
-        <v>19.76</v>
+        <v>21.56</v>
       </c>
       <c r="B322" t="n">
-        <v>2.21</v>
+        <v>3.66</v>
       </c>
       <c r="C322" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D322" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E322" t="inlineStr">
@@ -10414,7 +10414,7 @@
       </c>
       <c r="F322" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G322" t="n">
@@ -10423,10 +10423,10 @@
     </row>
     <row r="323">
       <c r="A323" t="n">
-        <v>19.09</v>
+        <v>28.87</v>
       </c>
       <c r="B323" t="n">
-        <v>3</v>
+        <v>3.67</v>
       </c>
       <c r="C323" t="inlineStr">
         <is>
@@ -10440,12 +10440,12 @@
       </c>
       <c r="E323" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F323" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G323" t="n">
@@ -10454,10 +10454,10 @@
     </row>
     <row r="324">
       <c r="A324" t="n">
-        <v>23.9</v>
+        <v>22.01</v>
       </c>
       <c r="B324" t="n">
-        <v>3.98</v>
+        <v>4</v>
       </c>
       <c r="C324" t="inlineStr">
         <is>
@@ -10480,19 +10480,19 @@
         </is>
       </c>
       <c r="G324" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="325">
       <c r="A325" t="n">
-        <v>25.89</v>
+        <v>19.76</v>
       </c>
       <c r="B325" t="n">
-        <v>3.89</v>
+        <v>2.21</v>
       </c>
       <c r="C325" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D325" t="inlineStr">
@@ -10507,7 +10507,7 @@
       </c>
       <c r="F325" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G325" t="n">
@@ -10516,10 +10516,10 @@
     </row>
     <row r="326">
       <c r="A326" t="n">
-        <v>20.09</v>
+        <v>19.09</v>
       </c>
       <c r="B326" t="n">
-        <v>20.96</v>
+        <v>3</v>
       </c>
       <c r="C326" t="inlineStr">
         <is>
@@ -10533,7 +10533,7 @@
       </c>
       <c r="E326" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F326" t="inlineStr">
@@ -10542,19 +10542,19 @@
         </is>
       </c>
       <c r="G326" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" t="n">
-        <v>14.56</v>
+        <v>23.9</v>
       </c>
       <c r="B327" t="n">
-        <v>2.78</v>
+        <v>3.98</v>
       </c>
       <c r="C327" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D327" t="inlineStr">
@@ -10564,24 +10564,24 @@
       </c>
       <c r="E327" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F327" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G327" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="328">
       <c r="A328" t="n">
-        <v>19.23</v>
+        <v>25.89</v>
       </c>
       <c r="B328" t="n">
-        <v>2.01</v>
+        <v>3.89</v>
       </c>
       <c r="C328" t="inlineStr">
         <is>
@@ -10609,10 +10609,10 @@
     </row>
     <row r="329">
       <c r="A329" t="n">
-        <v>28.45</v>
+        <v>20.09</v>
       </c>
       <c r="B329" t="n">
-        <v>2.45</v>
+        <v>20.96</v>
       </c>
       <c r="C329" t="inlineStr">
         <is>
@@ -10626,7 +10626,7 @@
       </c>
       <c r="E329" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F329" t="inlineStr">
@@ -10635,15 +10635,15 @@
         </is>
       </c>
       <c r="G329" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="330">
       <c r="A330" t="n">
-        <v>33.45</v>
+        <v>14.56</v>
       </c>
       <c r="B330" t="n">
-        <v>4.67</v>
+        <v>2.78</v>
       </c>
       <c r="C330" t="inlineStr">
         <is>
@@ -10666,19 +10666,19 @@
         </is>
       </c>
       <c r="G330" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="331">
       <c r="A331" t="n">
-        <v>24.67</v>
+        <v>19.23</v>
       </c>
       <c r="B331" t="n">
-        <v>2.5</v>
+        <v>2.01</v>
       </c>
       <c r="C331" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D331" t="inlineStr">
@@ -10688,7 +10688,7 @@
       </c>
       <c r="E331" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F331" t="inlineStr">
@@ -10702,10 +10702,10 @@
     </row>
     <row r="332">
       <c r="A332" t="n">
-        <v>26.9</v>
+        <v>28.45</v>
       </c>
       <c r="B332" t="n">
-        <v>3</v>
+        <v>2.45</v>
       </c>
       <c r="C332" t="inlineStr">
         <is>
@@ -10719,24 +10719,24 @@
       </c>
       <c r="E332" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F332" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G332" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="333">
       <c r="A333" t="n">
-        <v>17.6</v>
+        <v>33.45</v>
       </c>
       <c r="B333" t="n">
-        <v>2.5</v>
+        <v>4.67</v>
       </c>
       <c r="C333" t="inlineStr">
         <is>
@@ -10755,19 +10755,19 @@
       </c>
       <c r="F333" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G333" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="334">
       <c r="A334" t="n">
-        <v>21</v>
+        <v>24.67</v>
       </c>
       <c r="B334" t="n">
-        <v>2.6</v>
+        <v>2.5</v>
       </c>
       <c r="C334" t="inlineStr">
         <is>
@@ -10781,7 +10781,7 @@
       </c>
       <c r="E334" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F334" t="inlineStr">
@@ -10795,14 +10795,14 @@
     </row>
     <row r="335">
       <c r="A335" t="n">
-        <v>30.15</v>
+        <v>26.9</v>
       </c>
       <c r="B335" t="n">
         <v>3</v>
       </c>
       <c r="C335" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D335" t="inlineStr">
@@ -10812,24 +10812,24 @@
       </c>
       <c r="E335" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F335" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G335" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="336">
       <c r="A336" t="n">
-        <v>29.35</v>
+        <v>17.6</v>
       </c>
       <c r="B336" t="n">
-        <v>2.56</v>
+        <v>2.5</v>
       </c>
       <c r="C336" t="inlineStr">
         <is>
@@ -10848,7 +10848,7 @@
       </c>
       <c r="F336" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G336" t="n">
@@ -10857,14 +10857,14 @@
     </row>
     <row r="337">
       <c r="A337" t="n">
-        <v>31.5</v>
+        <v>21</v>
       </c>
       <c r="B337" t="n">
-        <v>3</v>
+        <v>2.6</v>
       </c>
       <c r="C337" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D337" t="inlineStr">
@@ -10874,7 +10874,7 @@
       </c>
       <c r="E337" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F337" t="inlineStr">
@@ -10888,10 +10888,10 @@
     </row>
     <row r="338">
       <c r="A338" t="n">
-        <v>14.69</v>
+        <v>30.15</v>
       </c>
       <c r="B338" t="n">
-        <v>1.5</v>
+        <v>3</v>
       </c>
       <c r="C338" t="inlineStr">
         <is>
@@ -10900,12 +10900,12 @@
       </c>
       <c r="D338" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E338" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F338" t="inlineStr">
@@ -10919,10 +10919,10 @@
     </row>
     <row r="339">
       <c r="A339" t="n">
-        <v>24</v>
+        <v>29.35</v>
       </c>
       <c r="B339" t="n">
-        <v>2.3</v>
+        <v>2.56</v>
       </c>
       <c r="C339" t="inlineStr">
         <is>
@@ -10931,12 +10931,12 @@
       </c>
       <c r="D339" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E339" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F339" t="inlineStr">
@@ -10945,15 +10945,15 @@
         </is>
       </c>
       <c r="G339" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="340">
       <c r="A340" t="n">
-        <v>26.35</v>
+        <v>31.5</v>
       </c>
       <c r="B340" t="n">
-        <v>2.59</v>
+        <v>3</v>
       </c>
       <c r="C340" t="inlineStr">
         <is>
@@ -10967,38 +10967,38 @@
       </c>
       <c r="E340" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F340" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G340" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="341">
       <c r="A341" t="n">
-        <v>16.65</v>
+        <v>14.69</v>
       </c>
       <c r="B341" t="n">
-        <v>2.94</v>
+        <v>1.5</v>
       </c>
       <c r="C341" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D341" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E341" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F341" t="inlineStr">
@@ -11007,29 +11007,29 @@
         </is>
       </c>
       <c r="G341" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="342">
       <c r="A342" t="n">
-        <v>21.56</v>
+        <v>24</v>
       </c>
       <c r="B342" t="n">
-        <v>3.34</v>
+        <v>2.3</v>
       </c>
       <c r="C342" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D342" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E342" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Friday</t>
         </is>
       </c>
       <c r="F342" t="inlineStr">
@@ -11043,10 +11043,10 @@
     </row>
     <row r="343">
       <c r="A343" t="n">
-        <v>25.68</v>
+        <v>26.35</v>
       </c>
       <c r="B343" t="n">
-        <v>2.78</v>
+        <v>2.59</v>
       </c>
       <c r="C343" t="inlineStr">
         <is>
@@ -11060,38 +11060,38 @@
       </c>
       <c r="E343" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F343" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G343" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="344">
       <c r="A344" t="n">
-        <v>22.33</v>
+        <v>16.65</v>
       </c>
       <c r="B344" t="n">
-        <v>3.9</v>
+        <v>2.94</v>
       </c>
       <c r="C344" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D344" t="inlineStr">
         <is>
-          <t>Yes</t>
+          <t>No</t>
         </is>
       </c>
       <c r="E344" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F344" t="inlineStr">
@@ -11100,24 +11100,24 @@
         </is>
       </c>
       <c r="G344" t="n">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="345">
       <c r="A345" t="n">
-        <v>18.67</v>
+        <v>21.56</v>
       </c>
       <c r="B345" t="n">
-        <v>2.09</v>
+        <v>3.34</v>
       </c>
       <c r="C345" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D345" t="inlineStr">
         <is>
-          <t>No</t>
+          <t>Yes</t>
         </is>
       </c>
       <c r="E345" t="inlineStr">
@@ -11127,7 +11127,7 @@
       </c>
       <c r="F345" t="inlineStr">
         <is>
-          <t>Dinner</t>
+          <t>Lunch</t>
         </is>
       </c>
       <c r="G345" t="n">
@@ -11136,10 +11136,10 @@
     </row>
     <row r="346">
       <c r="A346" t="n">
-        <v>18.09</v>
+        <v>25.68</v>
       </c>
       <c r="B346" t="n">
-        <v>3.45</v>
+        <v>2.78</v>
       </c>
       <c r="C346" t="inlineStr">
         <is>
@@ -11153,7 +11153,7 @@
       </c>
       <c r="E346" t="inlineStr">
         <is>
-          <t>Thursday</t>
+          <t>Sunday</t>
         </is>
       </c>
       <c r="F346" t="inlineStr">
@@ -11167,10 +11167,10 @@
     </row>
     <row r="347">
       <c r="A347" t="n">
-        <v>21.67</v>
+        <v>22.33</v>
       </c>
       <c r="B347" t="n">
-        <v>3</v>
+        <v>3.9</v>
       </c>
       <c r="C347" t="inlineStr">
         <is>
@@ -11198,14 +11198,14 @@
     </row>
     <row r="348">
       <c r="A348" t="n">
-        <v>27.23</v>
+        <v>18.67</v>
       </c>
       <c r="B348" t="n">
-        <v>2.9</v>
+        <v>2.09</v>
       </c>
       <c r="C348" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D348" t="inlineStr">
@@ -11215,12 +11215,12 @@
       </c>
       <c r="E348" t="inlineStr">
         <is>
-          <t>Friday</t>
+          <t>Saturday</t>
         </is>
       </c>
       <c r="F348" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G348" t="n">
@@ -11229,14 +11229,14 @@
     </row>
     <row r="349">
       <c r="A349" t="n">
-        <v>18.89</v>
+        <v>18.09</v>
       </c>
       <c r="B349" t="n">
-        <v>22.23</v>
+        <v>3.45</v>
       </c>
       <c r="C349" t="inlineStr">
         <is>
-          <t>Male</t>
+          <t>Female</t>
         </is>
       </c>
       <c r="D349" t="inlineStr">
@@ -11246,7 +11246,7 @@
       </c>
       <c r="E349" t="inlineStr">
         <is>
-          <t>Sunday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F349" t="inlineStr">
@@ -11255,19 +11255,19 @@
         </is>
       </c>
       <c r="G349" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="350">
       <c r="A350" t="n">
-        <v>16.37</v>
+        <v>21.67</v>
       </c>
       <c r="B350" t="n">
-        <v>3.21</v>
+        <v>3</v>
       </c>
       <c r="C350" t="inlineStr">
         <is>
-          <t>Female</t>
+          <t>Male</t>
         </is>
       </c>
       <c r="D350" t="inlineStr">
@@ -11277,46 +11277,139 @@
       </c>
       <c r="E350" t="inlineStr">
         <is>
-          <t>Saturday</t>
+          <t>Thursday</t>
         </is>
       </c>
       <c r="F350" t="inlineStr">
         <is>
-          <t>Lunch</t>
+          <t>Dinner</t>
         </is>
       </c>
       <c r="G350" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="351">
       <c r="A351" t="n">
+        <v>27.23</v>
+      </c>
+      <c r="B351" t="n">
+        <v>2.9</v>
+      </c>
+      <c r="C351" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D351" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E351" t="inlineStr">
+        <is>
+          <t>Friday</t>
+        </is>
+      </c>
+      <c r="F351" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
+      <c r="G351" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="n">
+        <v>18.89</v>
+      </c>
+      <c r="B352" t="n">
+        <v>22.23</v>
+      </c>
+      <c r="C352" t="inlineStr">
+        <is>
+          <t>Male</t>
+        </is>
+      </c>
+      <c r="D352" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E352" t="inlineStr">
+        <is>
+          <t>Sunday</t>
+        </is>
+      </c>
+      <c r="F352" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
+      <c r="G352" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="353">
+      <c r="A353" t="n">
+        <v>16.37</v>
+      </c>
+      <c r="B353" t="n">
+        <v>3.21</v>
+      </c>
+      <c r="C353" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D353" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="E353" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="F353" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
+      <c r="G353" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="354">
+      <c r="A354" t="n">
         <v>19.12</v>
       </c>
-      <c r="B351" t="n">
+      <c r="B354" t="n">
         <v>2.22</v>
       </c>
-      <c r="C351" t="inlineStr">
-        <is>
-          <t>Female</t>
-        </is>
-      </c>
-      <c r="D351" t="inlineStr">
-        <is>
-          <t>No</t>
-        </is>
-      </c>
-      <c r="E351" t="inlineStr">
-        <is>
-          <t>Saturday</t>
-        </is>
-      </c>
-      <c r="F351" t="inlineStr">
-        <is>
-          <t>Lunch</t>
-        </is>
-      </c>
-      <c r="G351" t="n">
+      <c r="C354" t="inlineStr">
+        <is>
+          <t>Female</t>
+        </is>
+      </c>
+      <c r="D354" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="E354" t="inlineStr">
+        <is>
+          <t>Saturday</t>
+        </is>
+      </c>
+      <c r="F354" t="inlineStr">
+        <is>
+          <t>Lunch</t>
+        </is>
+      </c>
+      <c r="G354" t="n">
         <v>4</v>
       </c>
     </row>

</xml_diff>